<commit_message>
Changing too test pyaugmecon instances results
</commit_message>
<xml_diff>
--- a/test/mokp/instances/2kp50.xlsx
+++ b/test/mokp/instances/2kp50.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/37609ee190385eca/Documentos/JosaFerreira/myJobs/02-projects/Jumento.jl/test/mokp/instances/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\whbles\pyaugmecon\tests\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{E1BC72FF-A24C-4F3D-8D0F-A910EAC8C8F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65EDE6B2-37D5-4966-88C6-D4F74257629D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BC72FF-A24C-4F3D-8D0F-A910EAC8C8F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="10455" windowHeight="10905" activeTab="1" xr2:uid="{DF6384DB-DFB1-4F3E-A725-F1DA5E529D8E}"/>
+    <workbookView xWindow="5010" yWindow="2595" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{DF6384DB-DFB1-4F3E-A725-F1DA5E529D8E}"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="2" r:id="rId1"/>
     <sheet name="b" sheetId="3" r:id="rId2"/>
     <sheet name="c" sheetId="1" r:id="rId3"/>
     <sheet name="payoff_table" sheetId="5" r:id="rId4"/>
-    <sheet name="pareto_sols" sheetId="4" r:id="rId5"/>
+    <sheet name="e_points" sheetId="6" r:id="rId5"/>
+    <sheet name="pareto_sols" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +72,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -87,7 +88,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -862,7 +863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CDD90C6-AFD3-4D3A-99B9-332F6F68C6C2}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1418,17 +1419,2988 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472D21B3-32B4-4C12-A7C7-63C45A248C7B}">
+  <dimension ref="A1:RY2"/>
+  <sheetViews>
+    <sheetView topLeftCell="RE1" workbookViewId="0">
+      <selection activeCell="RL4" sqref="RL4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:493" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+      <c r="N1">
+        <v>13</v>
+      </c>
+      <c r="O1">
+        <v>14</v>
+      </c>
+      <c r="P1">
+        <v>15</v>
+      </c>
+      <c r="Q1">
+        <v>16</v>
+      </c>
+      <c r="R1">
+        <v>17</v>
+      </c>
+      <c r="S1">
+        <v>18</v>
+      </c>
+      <c r="T1">
+        <v>19</v>
+      </c>
+      <c r="U1">
+        <v>20</v>
+      </c>
+      <c r="V1">
+        <v>21</v>
+      </c>
+      <c r="W1">
+        <v>22</v>
+      </c>
+      <c r="X1">
+        <v>23</v>
+      </c>
+      <c r="Y1">
+        <v>24</v>
+      </c>
+      <c r="Z1">
+        <v>25</v>
+      </c>
+      <c r="AA1">
+        <v>26</v>
+      </c>
+      <c r="AB1">
+        <v>27</v>
+      </c>
+      <c r="AC1">
+        <v>28</v>
+      </c>
+      <c r="AD1">
+        <v>29</v>
+      </c>
+      <c r="AE1">
+        <v>30</v>
+      </c>
+      <c r="AF1">
+        <v>31</v>
+      </c>
+      <c r="AG1">
+        <v>32</v>
+      </c>
+      <c r="AH1">
+        <v>33</v>
+      </c>
+      <c r="AI1">
+        <v>34</v>
+      </c>
+      <c r="AJ1">
+        <v>35</v>
+      </c>
+      <c r="AK1">
+        <v>36</v>
+      </c>
+      <c r="AL1">
+        <v>37</v>
+      </c>
+      <c r="AM1">
+        <v>38</v>
+      </c>
+      <c r="AN1">
+        <v>39</v>
+      </c>
+      <c r="AO1">
+        <v>40</v>
+      </c>
+      <c r="AP1">
+        <v>41</v>
+      </c>
+      <c r="AQ1">
+        <v>42</v>
+      </c>
+      <c r="AR1">
+        <v>43</v>
+      </c>
+      <c r="AS1">
+        <v>44</v>
+      </c>
+      <c r="AT1">
+        <v>45</v>
+      </c>
+      <c r="AU1">
+        <v>46</v>
+      </c>
+      <c r="AV1">
+        <v>47</v>
+      </c>
+      <c r="AW1">
+        <v>48</v>
+      </c>
+      <c r="AX1">
+        <v>49</v>
+      </c>
+      <c r="AY1">
+        <v>50</v>
+      </c>
+      <c r="AZ1">
+        <v>51</v>
+      </c>
+      <c r="BA1">
+        <v>52</v>
+      </c>
+      <c r="BB1">
+        <v>53</v>
+      </c>
+      <c r="BC1">
+        <v>54</v>
+      </c>
+      <c r="BD1">
+        <v>55</v>
+      </c>
+      <c r="BE1">
+        <v>56</v>
+      </c>
+      <c r="BF1">
+        <v>57</v>
+      </c>
+      <c r="BG1">
+        <v>58</v>
+      </c>
+      <c r="BH1">
+        <v>59</v>
+      </c>
+      <c r="BI1">
+        <v>60</v>
+      </c>
+      <c r="BJ1">
+        <v>61</v>
+      </c>
+      <c r="BK1">
+        <v>62</v>
+      </c>
+      <c r="BL1">
+        <v>63</v>
+      </c>
+      <c r="BM1">
+        <v>64</v>
+      </c>
+      <c r="BN1">
+        <v>65</v>
+      </c>
+      <c r="BO1">
+        <v>66</v>
+      </c>
+      <c r="BP1">
+        <v>67</v>
+      </c>
+      <c r="BQ1">
+        <v>68</v>
+      </c>
+      <c r="BR1">
+        <v>69</v>
+      </c>
+      <c r="BS1">
+        <v>70</v>
+      </c>
+      <c r="BT1">
+        <v>71</v>
+      </c>
+      <c r="BU1">
+        <v>72</v>
+      </c>
+      <c r="BV1">
+        <v>73</v>
+      </c>
+      <c r="BW1">
+        <v>74</v>
+      </c>
+      <c r="BX1">
+        <v>75</v>
+      </c>
+      <c r="BY1">
+        <v>76</v>
+      </c>
+      <c r="BZ1">
+        <v>77</v>
+      </c>
+      <c r="CA1">
+        <v>78</v>
+      </c>
+      <c r="CB1">
+        <v>79</v>
+      </c>
+      <c r="CC1">
+        <v>80</v>
+      </c>
+      <c r="CD1">
+        <v>81</v>
+      </c>
+      <c r="CE1">
+        <v>82</v>
+      </c>
+      <c r="CF1">
+        <v>83</v>
+      </c>
+      <c r="CG1">
+        <v>84</v>
+      </c>
+      <c r="CH1">
+        <v>85</v>
+      </c>
+      <c r="CI1">
+        <v>86</v>
+      </c>
+      <c r="CJ1">
+        <v>87</v>
+      </c>
+      <c r="CK1">
+        <v>88</v>
+      </c>
+      <c r="CL1">
+        <v>89</v>
+      </c>
+      <c r="CM1">
+        <v>90</v>
+      </c>
+      <c r="CN1">
+        <v>91</v>
+      </c>
+      <c r="CO1">
+        <v>92</v>
+      </c>
+      <c r="CP1">
+        <v>93</v>
+      </c>
+      <c r="CQ1">
+        <v>94</v>
+      </c>
+      <c r="CR1">
+        <v>95</v>
+      </c>
+      <c r="CS1">
+        <v>96</v>
+      </c>
+      <c r="CT1">
+        <v>97</v>
+      </c>
+      <c r="CU1">
+        <v>98</v>
+      </c>
+      <c r="CV1">
+        <v>99</v>
+      </c>
+      <c r="CW1">
+        <v>100</v>
+      </c>
+      <c r="CX1">
+        <v>101</v>
+      </c>
+      <c r="CY1">
+        <v>102</v>
+      </c>
+      <c r="CZ1">
+        <v>103</v>
+      </c>
+      <c r="DA1">
+        <v>104</v>
+      </c>
+      <c r="DB1">
+        <v>105</v>
+      </c>
+      <c r="DC1">
+        <v>106</v>
+      </c>
+      <c r="DD1">
+        <v>107</v>
+      </c>
+      <c r="DE1">
+        <v>108</v>
+      </c>
+      <c r="DF1">
+        <v>109</v>
+      </c>
+      <c r="DG1">
+        <v>110</v>
+      </c>
+      <c r="DH1">
+        <v>111</v>
+      </c>
+      <c r="DI1">
+        <v>112</v>
+      </c>
+      <c r="DJ1">
+        <v>113</v>
+      </c>
+      <c r="DK1">
+        <v>114</v>
+      </c>
+      <c r="DL1">
+        <v>115</v>
+      </c>
+      <c r="DM1">
+        <v>116</v>
+      </c>
+      <c r="DN1">
+        <v>117</v>
+      </c>
+      <c r="DO1">
+        <v>118</v>
+      </c>
+      <c r="DP1">
+        <v>119</v>
+      </c>
+      <c r="DQ1">
+        <v>120</v>
+      </c>
+      <c r="DR1">
+        <v>121</v>
+      </c>
+      <c r="DS1">
+        <v>122</v>
+      </c>
+      <c r="DT1">
+        <v>123</v>
+      </c>
+      <c r="DU1">
+        <v>124</v>
+      </c>
+      <c r="DV1">
+        <v>125</v>
+      </c>
+      <c r="DW1">
+        <v>126</v>
+      </c>
+      <c r="DX1">
+        <v>127</v>
+      </c>
+      <c r="DY1">
+        <v>128</v>
+      </c>
+      <c r="DZ1">
+        <v>129</v>
+      </c>
+      <c r="EA1">
+        <v>130</v>
+      </c>
+      <c r="EB1">
+        <v>131</v>
+      </c>
+      <c r="EC1">
+        <v>132</v>
+      </c>
+      <c r="ED1">
+        <v>133</v>
+      </c>
+      <c r="EE1">
+        <v>134</v>
+      </c>
+      <c r="EF1">
+        <v>135</v>
+      </c>
+      <c r="EG1">
+        <v>136</v>
+      </c>
+      <c r="EH1">
+        <v>137</v>
+      </c>
+      <c r="EI1">
+        <v>138</v>
+      </c>
+      <c r="EJ1">
+        <v>139</v>
+      </c>
+      <c r="EK1">
+        <v>140</v>
+      </c>
+      <c r="EL1">
+        <v>141</v>
+      </c>
+      <c r="EM1">
+        <v>142</v>
+      </c>
+      <c r="EN1">
+        <v>143</v>
+      </c>
+      <c r="EO1">
+        <v>144</v>
+      </c>
+      <c r="EP1">
+        <v>145</v>
+      </c>
+      <c r="EQ1">
+        <v>146</v>
+      </c>
+      <c r="ER1">
+        <v>147</v>
+      </c>
+      <c r="ES1">
+        <v>148</v>
+      </c>
+      <c r="ET1">
+        <v>149</v>
+      </c>
+      <c r="EU1">
+        <v>150</v>
+      </c>
+      <c r="EV1">
+        <v>151</v>
+      </c>
+      <c r="EW1">
+        <v>152</v>
+      </c>
+      <c r="EX1">
+        <v>153</v>
+      </c>
+      <c r="EY1">
+        <v>154</v>
+      </c>
+      <c r="EZ1">
+        <v>155</v>
+      </c>
+      <c r="FA1">
+        <v>156</v>
+      </c>
+      <c r="FB1">
+        <v>157</v>
+      </c>
+      <c r="FC1">
+        <v>158</v>
+      </c>
+      <c r="FD1">
+        <v>159</v>
+      </c>
+      <c r="FE1">
+        <v>160</v>
+      </c>
+      <c r="FF1">
+        <v>161</v>
+      </c>
+      <c r="FG1">
+        <v>162</v>
+      </c>
+      <c r="FH1">
+        <v>163</v>
+      </c>
+      <c r="FI1">
+        <v>164</v>
+      </c>
+      <c r="FJ1">
+        <v>165</v>
+      </c>
+      <c r="FK1">
+        <v>166</v>
+      </c>
+      <c r="FL1">
+        <v>167</v>
+      </c>
+      <c r="FM1">
+        <v>168</v>
+      </c>
+      <c r="FN1">
+        <v>169</v>
+      </c>
+      <c r="FO1">
+        <v>170</v>
+      </c>
+      <c r="FP1">
+        <v>171</v>
+      </c>
+      <c r="FQ1">
+        <v>172</v>
+      </c>
+      <c r="FR1">
+        <v>173</v>
+      </c>
+      <c r="FS1">
+        <v>174</v>
+      </c>
+      <c r="FT1">
+        <v>175</v>
+      </c>
+      <c r="FU1">
+        <v>176</v>
+      </c>
+      <c r="FV1">
+        <v>177</v>
+      </c>
+      <c r="FW1">
+        <v>178</v>
+      </c>
+      <c r="FX1">
+        <v>179</v>
+      </c>
+      <c r="FY1">
+        <v>180</v>
+      </c>
+      <c r="FZ1">
+        <v>181</v>
+      </c>
+      <c r="GA1">
+        <v>182</v>
+      </c>
+      <c r="GB1">
+        <v>183</v>
+      </c>
+      <c r="GC1">
+        <v>184</v>
+      </c>
+      <c r="GD1">
+        <v>185</v>
+      </c>
+      <c r="GE1">
+        <v>186</v>
+      </c>
+      <c r="GF1">
+        <v>187</v>
+      </c>
+      <c r="GG1">
+        <v>188</v>
+      </c>
+      <c r="GH1">
+        <v>189</v>
+      </c>
+      <c r="GI1">
+        <v>190</v>
+      </c>
+      <c r="GJ1">
+        <v>191</v>
+      </c>
+      <c r="GK1">
+        <v>192</v>
+      </c>
+      <c r="GL1">
+        <v>193</v>
+      </c>
+      <c r="GM1">
+        <v>194</v>
+      </c>
+      <c r="GN1">
+        <v>195</v>
+      </c>
+      <c r="GO1">
+        <v>196</v>
+      </c>
+      <c r="GP1">
+        <v>197</v>
+      </c>
+      <c r="GQ1">
+        <v>198</v>
+      </c>
+      <c r="GR1">
+        <v>199</v>
+      </c>
+      <c r="GS1">
+        <v>200</v>
+      </c>
+      <c r="GT1">
+        <v>201</v>
+      </c>
+      <c r="GU1">
+        <v>202</v>
+      </c>
+      <c r="GV1">
+        <v>203</v>
+      </c>
+      <c r="GW1">
+        <v>204</v>
+      </c>
+      <c r="GX1">
+        <v>205</v>
+      </c>
+      <c r="GY1">
+        <v>206</v>
+      </c>
+      <c r="GZ1">
+        <v>207</v>
+      </c>
+      <c r="HA1">
+        <v>208</v>
+      </c>
+      <c r="HB1">
+        <v>209</v>
+      </c>
+      <c r="HC1">
+        <v>210</v>
+      </c>
+      <c r="HD1">
+        <v>211</v>
+      </c>
+      <c r="HE1">
+        <v>212</v>
+      </c>
+      <c r="HF1">
+        <v>213</v>
+      </c>
+      <c r="HG1">
+        <v>214</v>
+      </c>
+      <c r="HH1">
+        <v>215</v>
+      </c>
+      <c r="HI1">
+        <v>216</v>
+      </c>
+      <c r="HJ1">
+        <v>217</v>
+      </c>
+      <c r="HK1">
+        <v>218</v>
+      </c>
+      <c r="HL1">
+        <v>219</v>
+      </c>
+      <c r="HM1">
+        <v>220</v>
+      </c>
+      <c r="HN1">
+        <v>221</v>
+      </c>
+      <c r="HO1">
+        <v>222</v>
+      </c>
+      <c r="HP1">
+        <v>223</v>
+      </c>
+      <c r="HQ1">
+        <v>224</v>
+      </c>
+      <c r="HR1">
+        <v>225</v>
+      </c>
+      <c r="HS1">
+        <v>226</v>
+      </c>
+      <c r="HT1">
+        <v>227</v>
+      </c>
+      <c r="HU1">
+        <v>228</v>
+      </c>
+      <c r="HV1">
+        <v>229</v>
+      </c>
+      <c r="HW1">
+        <v>230</v>
+      </c>
+      <c r="HX1">
+        <v>231</v>
+      </c>
+      <c r="HY1">
+        <v>232</v>
+      </c>
+      <c r="HZ1">
+        <v>233</v>
+      </c>
+      <c r="IA1">
+        <v>234</v>
+      </c>
+      <c r="IB1">
+        <v>235</v>
+      </c>
+      <c r="IC1">
+        <v>236</v>
+      </c>
+      <c r="ID1">
+        <v>237</v>
+      </c>
+      <c r="IE1">
+        <v>238</v>
+      </c>
+      <c r="IF1">
+        <v>239</v>
+      </c>
+      <c r="IG1">
+        <v>240</v>
+      </c>
+      <c r="IH1">
+        <v>241</v>
+      </c>
+      <c r="II1">
+        <v>242</v>
+      </c>
+      <c r="IJ1">
+        <v>243</v>
+      </c>
+      <c r="IK1">
+        <v>244</v>
+      </c>
+      <c r="IL1">
+        <v>245</v>
+      </c>
+      <c r="IM1">
+        <v>246</v>
+      </c>
+      <c r="IN1">
+        <v>247</v>
+      </c>
+      <c r="IO1">
+        <v>248</v>
+      </c>
+      <c r="IP1">
+        <v>249</v>
+      </c>
+      <c r="IQ1">
+        <v>250</v>
+      </c>
+      <c r="IR1">
+        <v>251</v>
+      </c>
+      <c r="IS1">
+        <v>252</v>
+      </c>
+      <c r="IT1">
+        <v>253</v>
+      </c>
+      <c r="IU1">
+        <v>254</v>
+      </c>
+      <c r="IV1">
+        <v>255</v>
+      </c>
+      <c r="IW1">
+        <v>256</v>
+      </c>
+      <c r="IX1">
+        <v>257</v>
+      </c>
+      <c r="IY1">
+        <v>258</v>
+      </c>
+      <c r="IZ1">
+        <v>259</v>
+      </c>
+      <c r="JA1">
+        <v>260</v>
+      </c>
+      <c r="JB1">
+        <v>261</v>
+      </c>
+      <c r="JC1">
+        <v>262</v>
+      </c>
+      <c r="JD1">
+        <v>263</v>
+      </c>
+      <c r="JE1">
+        <v>264</v>
+      </c>
+      <c r="JF1">
+        <v>265</v>
+      </c>
+      <c r="JG1">
+        <v>266</v>
+      </c>
+      <c r="JH1">
+        <v>267</v>
+      </c>
+      <c r="JI1">
+        <v>268</v>
+      </c>
+      <c r="JJ1">
+        <v>269</v>
+      </c>
+      <c r="JK1">
+        <v>270</v>
+      </c>
+      <c r="JL1">
+        <v>271</v>
+      </c>
+      <c r="JM1">
+        <v>272</v>
+      </c>
+      <c r="JN1">
+        <v>273</v>
+      </c>
+      <c r="JO1">
+        <v>274</v>
+      </c>
+      <c r="JP1">
+        <v>275</v>
+      </c>
+      <c r="JQ1">
+        <v>276</v>
+      </c>
+      <c r="JR1">
+        <v>277</v>
+      </c>
+      <c r="JS1">
+        <v>278</v>
+      </c>
+      <c r="JT1">
+        <v>279</v>
+      </c>
+      <c r="JU1">
+        <v>280</v>
+      </c>
+      <c r="JV1">
+        <v>281</v>
+      </c>
+      <c r="JW1">
+        <v>282</v>
+      </c>
+      <c r="JX1">
+        <v>283</v>
+      </c>
+      <c r="JY1">
+        <v>284</v>
+      </c>
+      <c r="JZ1">
+        <v>285</v>
+      </c>
+      <c r="KA1">
+        <v>286</v>
+      </c>
+      <c r="KB1">
+        <v>287</v>
+      </c>
+      <c r="KC1">
+        <v>288</v>
+      </c>
+      <c r="KD1">
+        <v>289</v>
+      </c>
+      <c r="KE1">
+        <v>290</v>
+      </c>
+      <c r="KF1">
+        <v>291</v>
+      </c>
+      <c r="KG1">
+        <v>292</v>
+      </c>
+      <c r="KH1">
+        <v>293</v>
+      </c>
+      <c r="KI1">
+        <v>294</v>
+      </c>
+      <c r="KJ1">
+        <v>295</v>
+      </c>
+      <c r="KK1">
+        <v>296</v>
+      </c>
+      <c r="KL1">
+        <v>297</v>
+      </c>
+      <c r="KM1">
+        <v>298</v>
+      </c>
+      <c r="KN1">
+        <v>299</v>
+      </c>
+      <c r="KO1">
+        <v>300</v>
+      </c>
+      <c r="KP1">
+        <v>301</v>
+      </c>
+      <c r="KQ1">
+        <v>302</v>
+      </c>
+      <c r="KR1">
+        <v>303</v>
+      </c>
+      <c r="KS1">
+        <v>304</v>
+      </c>
+      <c r="KT1">
+        <v>305</v>
+      </c>
+      <c r="KU1">
+        <v>306</v>
+      </c>
+      <c r="KV1">
+        <v>307</v>
+      </c>
+      <c r="KW1">
+        <v>308</v>
+      </c>
+      <c r="KX1">
+        <v>309</v>
+      </c>
+      <c r="KY1">
+        <v>310</v>
+      </c>
+      <c r="KZ1">
+        <v>311</v>
+      </c>
+      <c r="LA1">
+        <v>312</v>
+      </c>
+      <c r="LB1">
+        <v>313</v>
+      </c>
+      <c r="LC1">
+        <v>314</v>
+      </c>
+      <c r="LD1">
+        <v>315</v>
+      </c>
+      <c r="LE1">
+        <v>316</v>
+      </c>
+      <c r="LF1">
+        <v>317</v>
+      </c>
+      <c r="LG1">
+        <v>318</v>
+      </c>
+      <c r="LH1">
+        <v>319</v>
+      </c>
+      <c r="LI1">
+        <v>320</v>
+      </c>
+      <c r="LJ1">
+        <v>321</v>
+      </c>
+      <c r="LK1">
+        <v>322</v>
+      </c>
+      <c r="LL1">
+        <v>323</v>
+      </c>
+      <c r="LM1">
+        <v>324</v>
+      </c>
+      <c r="LN1">
+        <v>325</v>
+      </c>
+      <c r="LO1">
+        <v>326</v>
+      </c>
+      <c r="LP1">
+        <v>327</v>
+      </c>
+      <c r="LQ1">
+        <v>328</v>
+      </c>
+      <c r="LR1">
+        <v>329</v>
+      </c>
+      <c r="LS1">
+        <v>330</v>
+      </c>
+      <c r="LT1">
+        <v>331</v>
+      </c>
+      <c r="LU1">
+        <v>332</v>
+      </c>
+      <c r="LV1">
+        <v>333</v>
+      </c>
+      <c r="LW1">
+        <v>334</v>
+      </c>
+      <c r="LX1">
+        <v>335</v>
+      </c>
+      <c r="LY1">
+        <v>336</v>
+      </c>
+      <c r="LZ1">
+        <v>337</v>
+      </c>
+      <c r="MA1">
+        <v>338</v>
+      </c>
+      <c r="MB1">
+        <v>339</v>
+      </c>
+      <c r="MC1">
+        <v>340</v>
+      </c>
+      <c r="MD1">
+        <v>341</v>
+      </c>
+      <c r="ME1">
+        <v>342</v>
+      </c>
+      <c r="MF1">
+        <v>343</v>
+      </c>
+      <c r="MG1">
+        <v>344</v>
+      </c>
+      <c r="MH1">
+        <v>345</v>
+      </c>
+      <c r="MI1">
+        <v>346</v>
+      </c>
+      <c r="MJ1">
+        <v>347</v>
+      </c>
+      <c r="MK1">
+        <v>348</v>
+      </c>
+      <c r="ML1">
+        <v>349</v>
+      </c>
+      <c r="MM1">
+        <v>350</v>
+      </c>
+      <c r="MN1">
+        <v>351</v>
+      </c>
+      <c r="MO1">
+        <v>352</v>
+      </c>
+      <c r="MP1">
+        <v>353</v>
+      </c>
+      <c r="MQ1">
+        <v>354</v>
+      </c>
+      <c r="MR1">
+        <v>355</v>
+      </c>
+      <c r="MS1">
+        <v>356</v>
+      </c>
+      <c r="MT1">
+        <v>357</v>
+      </c>
+      <c r="MU1">
+        <v>358</v>
+      </c>
+      <c r="MV1">
+        <v>359</v>
+      </c>
+      <c r="MW1">
+        <v>360</v>
+      </c>
+      <c r="MX1">
+        <v>361</v>
+      </c>
+      <c r="MY1">
+        <v>362</v>
+      </c>
+      <c r="MZ1">
+        <v>363</v>
+      </c>
+      <c r="NA1">
+        <v>364</v>
+      </c>
+      <c r="NB1">
+        <v>365</v>
+      </c>
+      <c r="NC1">
+        <v>366</v>
+      </c>
+      <c r="ND1">
+        <v>367</v>
+      </c>
+      <c r="NE1">
+        <v>368</v>
+      </c>
+      <c r="NF1">
+        <v>369</v>
+      </c>
+      <c r="NG1">
+        <v>370</v>
+      </c>
+      <c r="NH1">
+        <v>371</v>
+      </c>
+      <c r="NI1">
+        <v>372</v>
+      </c>
+      <c r="NJ1">
+        <v>373</v>
+      </c>
+      <c r="NK1">
+        <v>374</v>
+      </c>
+      <c r="NL1">
+        <v>375</v>
+      </c>
+      <c r="NM1">
+        <v>376</v>
+      </c>
+      <c r="NN1">
+        <v>377</v>
+      </c>
+      <c r="NO1">
+        <v>378</v>
+      </c>
+      <c r="NP1">
+        <v>379</v>
+      </c>
+      <c r="NQ1">
+        <v>380</v>
+      </c>
+      <c r="NR1">
+        <v>381</v>
+      </c>
+      <c r="NS1">
+        <v>382</v>
+      </c>
+      <c r="NT1">
+        <v>383</v>
+      </c>
+      <c r="NU1">
+        <v>384</v>
+      </c>
+      <c r="NV1">
+        <v>385</v>
+      </c>
+      <c r="NW1">
+        <v>386</v>
+      </c>
+      <c r="NX1">
+        <v>387</v>
+      </c>
+      <c r="NY1">
+        <v>388</v>
+      </c>
+      <c r="NZ1">
+        <v>389</v>
+      </c>
+      <c r="OA1">
+        <v>390</v>
+      </c>
+      <c r="OB1">
+        <v>391</v>
+      </c>
+      <c r="OC1">
+        <v>392</v>
+      </c>
+      <c r="OD1">
+        <v>393</v>
+      </c>
+      <c r="OE1">
+        <v>394</v>
+      </c>
+      <c r="OF1">
+        <v>395</v>
+      </c>
+      <c r="OG1">
+        <v>396</v>
+      </c>
+      <c r="OH1">
+        <v>397</v>
+      </c>
+      <c r="OI1">
+        <v>398</v>
+      </c>
+      <c r="OJ1">
+        <v>399</v>
+      </c>
+      <c r="OK1">
+        <v>400</v>
+      </c>
+      <c r="OL1">
+        <v>401</v>
+      </c>
+      <c r="OM1">
+        <v>402</v>
+      </c>
+      <c r="ON1">
+        <v>403</v>
+      </c>
+      <c r="OO1">
+        <v>404</v>
+      </c>
+      <c r="OP1">
+        <v>405</v>
+      </c>
+      <c r="OQ1">
+        <v>406</v>
+      </c>
+      <c r="OR1">
+        <v>407</v>
+      </c>
+      <c r="OS1">
+        <v>408</v>
+      </c>
+      <c r="OT1">
+        <v>409</v>
+      </c>
+      <c r="OU1">
+        <v>410</v>
+      </c>
+      <c r="OV1">
+        <v>411</v>
+      </c>
+      <c r="OW1">
+        <v>412</v>
+      </c>
+      <c r="OX1">
+        <v>413</v>
+      </c>
+      <c r="OY1">
+        <v>414</v>
+      </c>
+      <c r="OZ1">
+        <v>415</v>
+      </c>
+      <c r="PA1">
+        <v>416</v>
+      </c>
+      <c r="PB1">
+        <v>417</v>
+      </c>
+      <c r="PC1">
+        <v>418</v>
+      </c>
+      <c r="PD1">
+        <v>419</v>
+      </c>
+      <c r="PE1">
+        <v>420</v>
+      </c>
+      <c r="PF1">
+        <v>421</v>
+      </c>
+      <c r="PG1">
+        <v>422</v>
+      </c>
+      <c r="PH1">
+        <v>423</v>
+      </c>
+      <c r="PI1">
+        <v>424</v>
+      </c>
+      <c r="PJ1">
+        <v>425</v>
+      </c>
+      <c r="PK1">
+        <v>426</v>
+      </c>
+      <c r="PL1">
+        <v>427</v>
+      </c>
+      <c r="PM1">
+        <v>428</v>
+      </c>
+      <c r="PN1">
+        <v>429</v>
+      </c>
+      <c r="PO1">
+        <v>430</v>
+      </c>
+      <c r="PP1">
+        <v>431</v>
+      </c>
+      <c r="PQ1">
+        <v>432</v>
+      </c>
+      <c r="PR1">
+        <v>433</v>
+      </c>
+      <c r="PS1">
+        <v>434</v>
+      </c>
+      <c r="PT1">
+        <v>435</v>
+      </c>
+      <c r="PU1">
+        <v>436</v>
+      </c>
+      <c r="PV1">
+        <v>437</v>
+      </c>
+      <c r="PW1">
+        <v>438</v>
+      </c>
+      <c r="PX1">
+        <v>439</v>
+      </c>
+      <c r="PY1">
+        <v>440</v>
+      </c>
+      <c r="PZ1">
+        <v>441</v>
+      </c>
+      <c r="QA1">
+        <v>442</v>
+      </c>
+      <c r="QB1">
+        <v>443</v>
+      </c>
+      <c r="QC1">
+        <v>444</v>
+      </c>
+      <c r="QD1">
+        <v>445</v>
+      </c>
+      <c r="QE1">
+        <v>446</v>
+      </c>
+      <c r="QF1">
+        <v>447</v>
+      </c>
+      <c r="QG1">
+        <v>448</v>
+      </c>
+      <c r="QH1">
+        <v>449</v>
+      </c>
+      <c r="QI1">
+        <v>450</v>
+      </c>
+      <c r="QJ1">
+        <v>451</v>
+      </c>
+      <c r="QK1">
+        <v>452</v>
+      </c>
+      <c r="QL1">
+        <v>453</v>
+      </c>
+      <c r="QM1">
+        <v>454</v>
+      </c>
+      <c r="QN1">
+        <v>455</v>
+      </c>
+      <c r="QO1">
+        <v>456</v>
+      </c>
+      <c r="QP1">
+        <v>457</v>
+      </c>
+      <c r="QQ1">
+        <v>458</v>
+      </c>
+      <c r="QR1">
+        <v>459</v>
+      </c>
+      <c r="QS1">
+        <v>460</v>
+      </c>
+      <c r="QT1">
+        <v>461</v>
+      </c>
+      <c r="QU1">
+        <v>462</v>
+      </c>
+      <c r="QV1">
+        <v>463</v>
+      </c>
+      <c r="QW1">
+        <v>464</v>
+      </c>
+      <c r="QX1">
+        <v>465</v>
+      </c>
+      <c r="QY1">
+        <v>466</v>
+      </c>
+      <c r="QZ1">
+        <v>467</v>
+      </c>
+      <c r="RA1">
+        <v>468</v>
+      </c>
+      <c r="RB1">
+        <v>469</v>
+      </c>
+      <c r="RC1">
+        <v>470</v>
+      </c>
+      <c r="RD1">
+        <v>471</v>
+      </c>
+      <c r="RE1">
+        <v>472</v>
+      </c>
+      <c r="RF1">
+        <v>473</v>
+      </c>
+      <c r="RG1">
+        <v>474</v>
+      </c>
+      <c r="RH1">
+        <v>475</v>
+      </c>
+      <c r="RI1">
+        <v>476</v>
+      </c>
+      <c r="RJ1">
+        <v>477</v>
+      </c>
+      <c r="RK1">
+        <v>478</v>
+      </c>
+      <c r="RL1">
+        <v>479</v>
+      </c>
+      <c r="RM1">
+        <v>480</v>
+      </c>
+      <c r="RN1">
+        <v>481</v>
+      </c>
+      <c r="RO1">
+        <v>482</v>
+      </c>
+      <c r="RP1">
+        <v>483</v>
+      </c>
+      <c r="RQ1">
+        <v>484</v>
+      </c>
+      <c r="RR1">
+        <v>485</v>
+      </c>
+      <c r="RS1">
+        <v>486</v>
+      </c>
+      <c r="RT1">
+        <v>487</v>
+      </c>
+      <c r="RU1">
+        <v>488</v>
+      </c>
+      <c r="RV1">
+        <v>489</v>
+      </c>
+      <c r="RW1">
+        <v>490</v>
+      </c>
+      <c r="RX1">
+        <v>491</v>
+      </c>
+      <c r="RY1">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="2" spans="1:493" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1529</v>
+      </c>
+      <c r="C2">
+        <v>1530</v>
+      </c>
+      <c r="D2">
+        <v>1531</v>
+      </c>
+      <c r="E2">
+        <v>1532</v>
+      </c>
+      <c r="F2">
+        <v>1533</v>
+      </c>
+      <c r="G2">
+        <v>1534</v>
+      </c>
+      <c r="H2">
+        <v>1535</v>
+      </c>
+      <c r="I2">
+        <v>1536</v>
+      </c>
+      <c r="J2">
+        <v>1537</v>
+      </c>
+      <c r="K2">
+        <v>1538</v>
+      </c>
+      <c r="L2">
+        <v>1539</v>
+      </c>
+      <c r="M2">
+        <v>1540</v>
+      </c>
+      <c r="N2">
+        <v>1541</v>
+      </c>
+      <c r="O2">
+        <v>1542</v>
+      </c>
+      <c r="P2">
+        <v>1543</v>
+      </c>
+      <c r="Q2">
+        <v>1544</v>
+      </c>
+      <c r="R2">
+        <v>1545</v>
+      </c>
+      <c r="S2">
+        <v>1546</v>
+      </c>
+      <c r="T2">
+        <v>1547</v>
+      </c>
+      <c r="U2">
+        <v>1548</v>
+      </c>
+      <c r="V2">
+        <v>1549</v>
+      </c>
+      <c r="W2">
+        <v>1550</v>
+      </c>
+      <c r="X2">
+        <v>1551</v>
+      </c>
+      <c r="Y2">
+        <v>1552</v>
+      </c>
+      <c r="Z2">
+        <v>1553</v>
+      </c>
+      <c r="AA2">
+        <v>1554</v>
+      </c>
+      <c r="AB2">
+        <v>1555</v>
+      </c>
+      <c r="AC2">
+        <v>1556</v>
+      </c>
+      <c r="AD2">
+        <v>1557</v>
+      </c>
+      <c r="AE2">
+        <v>1558</v>
+      </c>
+      <c r="AF2">
+        <v>1559</v>
+      </c>
+      <c r="AG2">
+        <v>1560</v>
+      </c>
+      <c r="AH2">
+        <v>1561</v>
+      </c>
+      <c r="AI2">
+        <v>1562</v>
+      </c>
+      <c r="AJ2">
+        <v>1563</v>
+      </c>
+      <c r="AK2">
+        <v>1564</v>
+      </c>
+      <c r="AL2">
+        <v>1565</v>
+      </c>
+      <c r="AM2">
+        <v>1566</v>
+      </c>
+      <c r="AN2">
+        <v>1567</v>
+      </c>
+      <c r="AO2">
+        <v>1568</v>
+      </c>
+      <c r="AP2">
+        <v>1569</v>
+      </c>
+      <c r="AQ2">
+        <v>1570</v>
+      </c>
+      <c r="AR2">
+        <v>1571</v>
+      </c>
+      <c r="AS2">
+        <v>1572</v>
+      </c>
+      <c r="AT2">
+        <v>1573</v>
+      </c>
+      <c r="AU2">
+        <v>1574</v>
+      </c>
+      <c r="AV2">
+        <v>1575</v>
+      </c>
+      <c r="AW2">
+        <v>1576</v>
+      </c>
+      <c r="AX2">
+        <v>1577</v>
+      </c>
+      <c r="AY2">
+        <v>1578</v>
+      </c>
+      <c r="AZ2">
+        <v>1579</v>
+      </c>
+      <c r="BA2">
+        <v>1580</v>
+      </c>
+      <c r="BB2">
+        <v>1581</v>
+      </c>
+      <c r="BC2">
+        <v>1582</v>
+      </c>
+      <c r="BD2">
+        <v>1583</v>
+      </c>
+      <c r="BE2">
+        <v>1584</v>
+      </c>
+      <c r="BF2">
+        <v>1585</v>
+      </c>
+      <c r="BG2">
+        <v>1586</v>
+      </c>
+      <c r="BH2">
+        <v>1587</v>
+      </c>
+      <c r="BI2">
+        <v>1588</v>
+      </c>
+      <c r="BJ2">
+        <v>1589</v>
+      </c>
+      <c r="BK2">
+        <v>1590</v>
+      </c>
+      <c r="BL2">
+        <v>1591</v>
+      </c>
+      <c r="BM2">
+        <v>1592</v>
+      </c>
+      <c r="BN2">
+        <v>1593</v>
+      </c>
+      <c r="BO2">
+        <v>1594</v>
+      </c>
+      <c r="BP2">
+        <v>1595</v>
+      </c>
+      <c r="BQ2">
+        <v>1596</v>
+      </c>
+      <c r="BR2">
+        <v>1597</v>
+      </c>
+      <c r="BS2">
+        <v>1598</v>
+      </c>
+      <c r="BT2">
+        <v>1599</v>
+      </c>
+      <c r="BU2">
+        <v>1600</v>
+      </c>
+      <c r="BV2">
+        <v>1601</v>
+      </c>
+      <c r="BW2">
+        <v>1602</v>
+      </c>
+      <c r="BX2">
+        <v>1603</v>
+      </c>
+      <c r="BY2">
+        <v>1604</v>
+      </c>
+      <c r="BZ2">
+        <v>1605</v>
+      </c>
+      <c r="CA2">
+        <v>1606</v>
+      </c>
+      <c r="CB2">
+        <v>1607</v>
+      </c>
+      <c r="CC2">
+        <v>1608</v>
+      </c>
+      <c r="CD2">
+        <v>1609</v>
+      </c>
+      <c r="CE2">
+        <v>1610</v>
+      </c>
+      <c r="CF2">
+        <v>1611</v>
+      </c>
+      <c r="CG2">
+        <v>1612</v>
+      </c>
+      <c r="CH2">
+        <v>1613</v>
+      </c>
+      <c r="CI2">
+        <v>1614</v>
+      </c>
+      <c r="CJ2">
+        <v>1615</v>
+      </c>
+      <c r="CK2">
+        <v>1616</v>
+      </c>
+      <c r="CL2">
+        <v>1617</v>
+      </c>
+      <c r="CM2">
+        <v>1618</v>
+      </c>
+      <c r="CN2">
+        <v>1619</v>
+      </c>
+      <c r="CO2">
+        <v>1620</v>
+      </c>
+      <c r="CP2">
+        <v>1621</v>
+      </c>
+      <c r="CQ2">
+        <v>1622</v>
+      </c>
+      <c r="CR2">
+        <v>1623</v>
+      </c>
+      <c r="CS2">
+        <v>1624</v>
+      </c>
+      <c r="CT2">
+        <v>1625</v>
+      </c>
+      <c r="CU2">
+        <v>1626</v>
+      </c>
+      <c r="CV2">
+        <v>1627</v>
+      </c>
+      <c r="CW2">
+        <v>1628</v>
+      </c>
+      <c r="CX2">
+        <v>1629</v>
+      </c>
+      <c r="CY2">
+        <v>1630</v>
+      </c>
+      <c r="CZ2">
+        <v>1631</v>
+      </c>
+      <c r="DA2">
+        <v>1632</v>
+      </c>
+      <c r="DB2">
+        <v>1633</v>
+      </c>
+      <c r="DC2">
+        <v>1634</v>
+      </c>
+      <c r="DD2">
+        <v>1635</v>
+      </c>
+      <c r="DE2">
+        <v>1636</v>
+      </c>
+      <c r="DF2">
+        <v>1637</v>
+      </c>
+      <c r="DG2">
+        <v>1638</v>
+      </c>
+      <c r="DH2">
+        <v>1639</v>
+      </c>
+      <c r="DI2">
+        <v>1640</v>
+      </c>
+      <c r="DJ2">
+        <v>1641</v>
+      </c>
+      <c r="DK2">
+        <v>1642</v>
+      </c>
+      <c r="DL2">
+        <v>1643</v>
+      </c>
+      <c r="DM2">
+        <v>1644</v>
+      </c>
+      <c r="DN2">
+        <v>1645</v>
+      </c>
+      <c r="DO2">
+        <v>1646</v>
+      </c>
+      <c r="DP2">
+        <v>1647</v>
+      </c>
+      <c r="DQ2">
+        <v>1648</v>
+      </c>
+      <c r="DR2">
+        <v>1649</v>
+      </c>
+      <c r="DS2">
+        <v>1650</v>
+      </c>
+      <c r="DT2">
+        <v>1651</v>
+      </c>
+      <c r="DU2">
+        <v>1652</v>
+      </c>
+      <c r="DV2">
+        <v>1653</v>
+      </c>
+      <c r="DW2">
+        <v>1654</v>
+      </c>
+      <c r="DX2">
+        <v>1655</v>
+      </c>
+      <c r="DY2">
+        <v>1656</v>
+      </c>
+      <c r="DZ2">
+        <v>1657</v>
+      </c>
+      <c r="EA2">
+        <v>1658</v>
+      </c>
+      <c r="EB2">
+        <v>1659</v>
+      </c>
+      <c r="EC2">
+        <v>1660</v>
+      </c>
+      <c r="ED2">
+        <v>1661</v>
+      </c>
+      <c r="EE2">
+        <v>1662</v>
+      </c>
+      <c r="EF2">
+        <v>1663</v>
+      </c>
+      <c r="EG2">
+        <v>1664</v>
+      </c>
+      <c r="EH2">
+        <v>1665</v>
+      </c>
+      <c r="EI2">
+        <v>1666</v>
+      </c>
+      <c r="EJ2">
+        <v>1667</v>
+      </c>
+      <c r="EK2">
+        <v>1668</v>
+      </c>
+      <c r="EL2">
+        <v>1669</v>
+      </c>
+      <c r="EM2">
+        <v>1670</v>
+      </c>
+      <c r="EN2">
+        <v>1671</v>
+      </c>
+      <c r="EO2">
+        <v>1672</v>
+      </c>
+      <c r="EP2">
+        <v>1673</v>
+      </c>
+      <c r="EQ2">
+        <v>1674</v>
+      </c>
+      <c r="ER2">
+        <v>1675</v>
+      </c>
+      <c r="ES2">
+        <v>1676</v>
+      </c>
+      <c r="ET2">
+        <v>1677</v>
+      </c>
+      <c r="EU2">
+        <v>1678</v>
+      </c>
+      <c r="EV2">
+        <v>1679</v>
+      </c>
+      <c r="EW2">
+        <v>1680</v>
+      </c>
+      <c r="EX2">
+        <v>1681</v>
+      </c>
+      <c r="EY2">
+        <v>1682</v>
+      </c>
+      <c r="EZ2">
+        <v>1683</v>
+      </c>
+      <c r="FA2">
+        <v>1684</v>
+      </c>
+      <c r="FB2">
+        <v>1685</v>
+      </c>
+      <c r="FC2">
+        <v>1686</v>
+      </c>
+      <c r="FD2">
+        <v>1687</v>
+      </c>
+      <c r="FE2">
+        <v>1688</v>
+      </c>
+      <c r="FF2">
+        <v>1689</v>
+      </c>
+      <c r="FG2">
+        <v>1690</v>
+      </c>
+      <c r="FH2">
+        <v>1691</v>
+      </c>
+      <c r="FI2">
+        <v>1692</v>
+      </c>
+      <c r="FJ2">
+        <v>1693</v>
+      </c>
+      <c r="FK2">
+        <v>1694</v>
+      </c>
+      <c r="FL2">
+        <v>1695</v>
+      </c>
+      <c r="FM2">
+        <v>1696</v>
+      </c>
+      <c r="FN2">
+        <v>1697</v>
+      </c>
+      <c r="FO2">
+        <v>1698</v>
+      </c>
+      <c r="FP2">
+        <v>1699</v>
+      </c>
+      <c r="FQ2">
+        <v>1700</v>
+      </c>
+      <c r="FR2">
+        <v>1701</v>
+      </c>
+      <c r="FS2">
+        <v>1702</v>
+      </c>
+      <c r="FT2">
+        <v>1703</v>
+      </c>
+      <c r="FU2">
+        <v>1704</v>
+      </c>
+      <c r="FV2">
+        <v>1705</v>
+      </c>
+      <c r="FW2">
+        <v>1706</v>
+      </c>
+      <c r="FX2">
+        <v>1707</v>
+      </c>
+      <c r="FY2">
+        <v>1708</v>
+      </c>
+      <c r="FZ2">
+        <v>1709</v>
+      </c>
+      <c r="GA2">
+        <v>1710</v>
+      </c>
+      <c r="GB2">
+        <v>1711</v>
+      </c>
+      <c r="GC2">
+        <v>1712</v>
+      </c>
+      <c r="GD2">
+        <v>1713</v>
+      </c>
+      <c r="GE2">
+        <v>1714</v>
+      </c>
+      <c r="GF2">
+        <v>1715</v>
+      </c>
+      <c r="GG2">
+        <v>1716</v>
+      </c>
+      <c r="GH2">
+        <v>1717</v>
+      </c>
+      <c r="GI2">
+        <v>1718</v>
+      </c>
+      <c r="GJ2">
+        <v>1719</v>
+      </c>
+      <c r="GK2">
+        <v>1720</v>
+      </c>
+      <c r="GL2">
+        <v>1721</v>
+      </c>
+      <c r="GM2">
+        <v>1722</v>
+      </c>
+      <c r="GN2">
+        <v>1723</v>
+      </c>
+      <c r="GO2">
+        <v>1724</v>
+      </c>
+      <c r="GP2">
+        <v>1725</v>
+      </c>
+      <c r="GQ2">
+        <v>1726</v>
+      </c>
+      <c r="GR2">
+        <v>1727</v>
+      </c>
+      <c r="GS2">
+        <v>1728</v>
+      </c>
+      <c r="GT2">
+        <v>1729</v>
+      </c>
+      <c r="GU2">
+        <v>1730</v>
+      </c>
+      <c r="GV2">
+        <v>1731</v>
+      </c>
+      <c r="GW2">
+        <v>1732</v>
+      </c>
+      <c r="GX2">
+        <v>1733</v>
+      </c>
+      <c r="GY2">
+        <v>1734</v>
+      </c>
+      <c r="GZ2">
+        <v>1735</v>
+      </c>
+      <c r="HA2">
+        <v>1736</v>
+      </c>
+      <c r="HB2">
+        <v>1737</v>
+      </c>
+      <c r="HC2">
+        <v>1738</v>
+      </c>
+      <c r="HD2">
+        <v>1739</v>
+      </c>
+      <c r="HE2">
+        <v>1740</v>
+      </c>
+      <c r="HF2">
+        <v>1741</v>
+      </c>
+      <c r="HG2">
+        <v>1742</v>
+      </c>
+      <c r="HH2">
+        <v>1743</v>
+      </c>
+      <c r="HI2">
+        <v>1744</v>
+      </c>
+      <c r="HJ2">
+        <v>1745</v>
+      </c>
+      <c r="HK2">
+        <v>1746</v>
+      </c>
+      <c r="HL2">
+        <v>1747</v>
+      </c>
+      <c r="HM2">
+        <v>1748</v>
+      </c>
+      <c r="HN2">
+        <v>1749</v>
+      </c>
+      <c r="HO2">
+        <v>1750</v>
+      </c>
+      <c r="HP2">
+        <v>1751</v>
+      </c>
+      <c r="HQ2">
+        <v>1752</v>
+      </c>
+      <c r="HR2">
+        <v>1753</v>
+      </c>
+      <c r="HS2">
+        <v>1754</v>
+      </c>
+      <c r="HT2">
+        <v>1755</v>
+      </c>
+      <c r="HU2">
+        <v>1756</v>
+      </c>
+      <c r="HV2">
+        <v>1757</v>
+      </c>
+      <c r="HW2">
+        <v>1758</v>
+      </c>
+      <c r="HX2">
+        <v>1759</v>
+      </c>
+      <c r="HY2">
+        <v>1760</v>
+      </c>
+      <c r="HZ2">
+        <v>1761</v>
+      </c>
+      <c r="IA2">
+        <v>1762</v>
+      </c>
+      <c r="IB2">
+        <v>1763</v>
+      </c>
+      <c r="IC2">
+        <v>1764</v>
+      </c>
+      <c r="ID2">
+        <v>1765</v>
+      </c>
+      <c r="IE2">
+        <v>1766</v>
+      </c>
+      <c r="IF2">
+        <v>1767</v>
+      </c>
+      <c r="IG2">
+        <v>1768</v>
+      </c>
+      <c r="IH2">
+        <v>1769</v>
+      </c>
+      <c r="II2">
+        <v>1770</v>
+      </c>
+      <c r="IJ2">
+        <v>1771</v>
+      </c>
+      <c r="IK2">
+        <v>1772</v>
+      </c>
+      <c r="IL2">
+        <v>1773</v>
+      </c>
+      <c r="IM2">
+        <v>1774</v>
+      </c>
+      <c r="IN2">
+        <v>1775</v>
+      </c>
+      <c r="IO2">
+        <v>1776</v>
+      </c>
+      <c r="IP2">
+        <v>1777</v>
+      </c>
+      <c r="IQ2">
+        <v>1778</v>
+      </c>
+      <c r="IR2">
+        <v>1779</v>
+      </c>
+      <c r="IS2">
+        <v>1780</v>
+      </c>
+      <c r="IT2">
+        <v>1781</v>
+      </c>
+      <c r="IU2">
+        <v>1782</v>
+      </c>
+      <c r="IV2">
+        <v>1783</v>
+      </c>
+      <c r="IW2">
+        <v>1784</v>
+      </c>
+      <c r="IX2">
+        <v>1785</v>
+      </c>
+      <c r="IY2">
+        <v>1786</v>
+      </c>
+      <c r="IZ2">
+        <v>1787</v>
+      </c>
+      <c r="JA2">
+        <v>1788</v>
+      </c>
+      <c r="JB2">
+        <v>1789</v>
+      </c>
+      <c r="JC2">
+        <v>1790</v>
+      </c>
+      <c r="JD2">
+        <v>1791</v>
+      </c>
+      <c r="JE2">
+        <v>1792</v>
+      </c>
+      <c r="JF2">
+        <v>1793</v>
+      </c>
+      <c r="JG2">
+        <v>1794</v>
+      </c>
+      <c r="JH2">
+        <v>1795</v>
+      </c>
+      <c r="JI2">
+        <v>1796</v>
+      </c>
+      <c r="JJ2">
+        <v>1797</v>
+      </c>
+      <c r="JK2">
+        <v>1798</v>
+      </c>
+      <c r="JL2">
+        <v>1799</v>
+      </c>
+      <c r="JM2">
+        <v>1800</v>
+      </c>
+      <c r="JN2">
+        <v>1801</v>
+      </c>
+      <c r="JO2">
+        <v>1802</v>
+      </c>
+      <c r="JP2">
+        <v>1803</v>
+      </c>
+      <c r="JQ2">
+        <v>1804</v>
+      </c>
+      <c r="JR2">
+        <v>1805</v>
+      </c>
+      <c r="JS2">
+        <v>1806</v>
+      </c>
+      <c r="JT2">
+        <v>1807</v>
+      </c>
+      <c r="JU2">
+        <v>1808</v>
+      </c>
+      <c r="JV2">
+        <v>1809</v>
+      </c>
+      <c r="JW2">
+        <v>1810</v>
+      </c>
+      <c r="JX2">
+        <v>1811</v>
+      </c>
+      <c r="JY2">
+        <v>1812</v>
+      </c>
+      <c r="JZ2">
+        <v>1813</v>
+      </c>
+      <c r="KA2">
+        <v>1814</v>
+      </c>
+      <c r="KB2">
+        <v>1815</v>
+      </c>
+      <c r="KC2">
+        <v>1816</v>
+      </c>
+      <c r="KD2">
+        <v>1817</v>
+      </c>
+      <c r="KE2">
+        <v>1818</v>
+      </c>
+      <c r="KF2">
+        <v>1819</v>
+      </c>
+      <c r="KG2">
+        <v>1820</v>
+      </c>
+      <c r="KH2">
+        <v>1821</v>
+      </c>
+      <c r="KI2">
+        <v>1822</v>
+      </c>
+      <c r="KJ2">
+        <v>1823</v>
+      </c>
+      <c r="KK2">
+        <v>1824</v>
+      </c>
+      <c r="KL2">
+        <v>1825</v>
+      </c>
+      <c r="KM2">
+        <v>1826</v>
+      </c>
+      <c r="KN2">
+        <v>1827</v>
+      </c>
+      <c r="KO2">
+        <v>1828</v>
+      </c>
+      <c r="KP2">
+        <v>1829</v>
+      </c>
+      <c r="KQ2">
+        <v>1830</v>
+      </c>
+      <c r="KR2">
+        <v>1831</v>
+      </c>
+      <c r="KS2">
+        <v>1832</v>
+      </c>
+      <c r="KT2">
+        <v>1833</v>
+      </c>
+      <c r="KU2">
+        <v>1834</v>
+      </c>
+      <c r="KV2">
+        <v>1835</v>
+      </c>
+      <c r="KW2">
+        <v>1836</v>
+      </c>
+      <c r="KX2">
+        <v>1837</v>
+      </c>
+      <c r="KY2">
+        <v>1838</v>
+      </c>
+      <c r="KZ2">
+        <v>1839</v>
+      </c>
+      <c r="LA2">
+        <v>1840</v>
+      </c>
+      <c r="LB2">
+        <v>1841</v>
+      </c>
+      <c r="LC2">
+        <v>1842</v>
+      </c>
+      <c r="LD2">
+        <v>1843</v>
+      </c>
+      <c r="LE2">
+        <v>1844</v>
+      </c>
+      <c r="LF2">
+        <v>1845</v>
+      </c>
+      <c r="LG2">
+        <v>1846</v>
+      </c>
+      <c r="LH2">
+        <v>1847</v>
+      </c>
+      <c r="LI2">
+        <v>1848</v>
+      </c>
+      <c r="LJ2">
+        <v>1849</v>
+      </c>
+      <c r="LK2">
+        <v>1850</v>
+      </c>
+      <c r="LL2">
+        <v>1851</v>
+      </c>
+      <c r="LM2">
+        <v>1852</v>
+      </c>
+      <c r="LN2">
+        <v>1853</v>
+      </c>
+      <c r="LO2">
+        <v>1854</v>
+      </c>
+      <c r="LP2">
+        <v>1855</v>
+      </c>
+      <c r="LQ2">
+        <v>1856</v>
+      </c>
+      <c r="LR2">
+        <v>1857</v>
+      </c>
+      <c r="LS2">
+        <v>1858</v>
+      </c>
+      <c r="LT2">
+        <v>1859</v>
+      </c>
+      <c r="LU2">
+        <v>1860</v>
+      </c>
+      <c r="LV2">
+        <v>1861</v>
+      </c>
+      <c r="LW2">
+        <v>1862</v>
+      </c>
+      <c r="LX2">
+        <v>1863</v>
+      </c>
+      <c r="LY2">
+        <v>1864</v>
+      </c>
+      <c r="LZ2">
+        <v>1865</v>
+      </c>
+      <c r="MA2">
+        <v>1866</v>
+      </c>
+      <c r="MB2">
+        <v>1867</v>
+      </c>
+      <c r="MC2">
+        <v>1868</v>
+      </c>
+      <c r="MD2">
+        <v>1869</v>
+      </c>
+      <c r="ME2">
+        <v>1870</v>
+      </c>
+      <c r="MF2">
+        <v>1871</v>
+      </c>
+      <c r="MG2">
+        <v>1872</v>
+      </c>
+      <c r="MH2">
+        <v>1873</v>
+      </c>
+      <c r="MI2">
+        <v>1874</v>
+      </c>
+      <c r="MJ2">
+        <v>1875</v>
+      </c>
+      <c r="MK2">
+        <v>1876</v>
+      </c>
+      <c r="ML2">
+        <v>1877</v>
+      </c>
+      <c r="MM2">
+        <v>1878</v>
+      </c>
+      <c r="MN2">
+        <v>1879</v>
+      </c>
+      <c r="MO2">
+        <v>1880</v>
+      </c>
+      <c r="MP2">
+        <v>1881</v>
+      </c>
+      <c r="MQ2">
+        <v>1882</v>
+      </c>
+      <c r="MR2">
+        <v>1883</v>
+      </c>
+      <c r="MS2">
+        <v>1884</v>
+      </c>
+      <c r="MT2">
+        <v>1885</v>
+      </c>
+      <c r="MU2">
+        <v>1886</v>
+      </c>
+      <c r="MV2">
+        <v>1887</v>
+      </c>
+      <c r="MW2">
+        <v>1888</v>
+      </c>
+      <c r="MX2">
+        <v>1889</v>
+      </c>
+      <c r="MY2">
+        <v>1890</v>
+      </c>
+      <c r="MZ2">
+        <v>1891</v>
+      </c>
+      <c r="NA2">
+        <v>1892</v>
+      </c>
+      <c r="NB2">
+        <v>1893</v>
+      </c>
+      <c r="NC2">
+        <v>1894</v>
+      </c>
+      <c r="ND2">
+        <v>1895</v>
+      </c>
+      <c r="NE2">
+        <v>1896</v>
+      </c>
+      <c r="NF2">
+        <v>1897</v>
+      </c>
+      <c r="NG2">
+        <v>1898</v>
+      </c>
+      <c r="NH2">
+        <v>1899</v>
+      </c>
+      <c r="NI2">
+        <v>1900</v>
+      </c>
+      <c r="NJ2">
+        <v>1901</v>
+      </c>
+      <c r="NK2">
+        <v>1902</v>
+      </c>
+      <c r="NL2">
+        <v>1903</v>
+      </c>
+      <c r="NM2">
+        <v>1904</v>
+      </c>
+      <c r="NN2">
+        <v>1905</v>
+      </c>
+      <c r="NO2">
+        <v>1906</v>
+      </c>
+      <c r="NP2">
+        <v>1907</v>
+      </c>
+      <c r="NQ2">
+        <v>1908</v>
+      </c>
+      <c r="NR2">
+        <v>1909</v>
+      </c>
+      <c r="NS2">
+        <v>1910</v>
+      </c>
+      <c r="NT2">
+        <v>1911</v>
+      </c>
+      <c r="NU2">
+        <v>1912</v>
+      </c>
+      <c r="NV2">
+        <v>1913</v>
+      </c>
+      <c r="NW2">
+        <v>1914</v>
+      </c>
+      <c r="NX2">
+        <v>1915</v>
+      </c>
+      <c r="NY2">
+        <v>1916</v>
+      </c>
+      <c r="NZ2">
+        <v>1917</v>
+      </c>
+      <c r="OA2">
+        <v>1918</v>
+      </c>
+      <c r="OB2">
+        <v>1919</v>
+      </c>
+      <c r="OC2">
+        <v>1920</v>
+      </c>
+      <c r="OD2">
+        <v>1921</v>
+      </c>
+      <c r="OE2">
+        <v>1922</v>
+      </c>
+      <c r="OF2">
+        <v>1923</v>
+      </c>
+      <c r="OG2">
+        <v>1924</v>
+      </c>
+      <c r="OH2">
+        <v>1925</v>
+      </c>
+      <c r="OI2">
+        <v>1926</v>
+      </c>
+      <c r="OJ2">
+        <v>1927</v>
+      </c>
+      <c r="OK2">
+        <v>1928</v>
+      </c>
+      <c r="OL2">
+        <v>1929</v>
+      </c>
+      <c r="OM2">
+        <v>1930</v>
+      </c>
+      <c r="ON2">
+        <v>1931</v>
+      </c>
+      <c r="OO2">
+        <v>1932</v>
+      </c>
+      <c r="OP2">
+        <v>1933</v>
+      </c>
+      <c r="OQ2">
+        <v>1934</v>
+      </c>
+      <c r="OR2">
+        <v>1935</v>
+      </c>
+      <c r="OS2">
+        <v>1936</v>
+      </c>
+      <c r="OT2">
+        <v>1937</v>
+      </c>
+      <c r="OU2">
+        <v>1938</v>
+      </c>
+      <c r="OV2">
+        <v>1939</v>
+      </c>
+      <c r="OW2">
+        <v>1940</v>
+      </c>
+      <c r="OX2">
+        <v>1941</v>
+      </c>
+      <c r="OY2">
+        <v>1942</v>
+      </c>
+      <c r="OZ2">
+        <v>1943</v>
+      </c>
+      <c r="PA2">
+        <v>1944</v>
+      </c>
+      <c r="PB2">
+        <v>1945</v>
+      </c>
+      <c r="PC2">
+        <v>1946</v>
+      </c>
+      <c r="PD2">
+        <v>1947</v>
+      </c>
+      <c r="PE2">
+        <v>1948</v>
+      </c>
+      <c r="PF2">
+        <v>1949</v>
+      </c>
+      <c r="PG2">
+        <v>1950</v>
+      </c>
+      <c r="PH2">
+        <v>1951</v>
+      </c>
+      <c r="PI2">
+        <v>1952</v>
+      </c>
+      <c r="PJ2">
+        <v>1953</v>
+      </c>
+      <c r="PK2">
+        <v>1954</v>
+      </c>
+      <c r="PL2">
+        <v>1955</v>
+      </c>
+      <c r="PM2">
+        <v>1956</v>
+      </c>
+      <c r="PN2">
+        <v>1957</v>
+      </c>
+      <c r="PO2">
+        <v>1958</v>
+      </c>
+      <c r="PP2">
+        <v>1959</v>
+      </c>
+      <c r="PQ2">
+        <v>1960</v>
+      </c>
+      <c r="PR2">
+        <v>1961</v>
+      </c>
+      <c r="PS2">
+        <v>1962</v>
+      </c>
+      <c r="PT2">
+        <v>1963</v>
+      </c>
+      <c r="PU2">
+        <v>1964</v>
+      </c>
+      <c r="PV2">
+        <v>1965</v>
+      </c>
+      <c r="PW2">
+        <v>1966</v>
+      </c>
+      <c r="PX2">
+        <v>1967</v>
+      </c>
+      <c r="PY2">
+        <v>1968</v>
+      </c>
+      <c r="PZ2">
+        <v>1969</v>
+      </c>
+      <c r="QA2">
+        <v>1970</v>
+      </c>
+      <c r="QB2">
+        <v>1971</v>
+      </c>
+      <c r="QC2">
+        <v>1972</v>
+      </c>
+      <c r="QD2">
+        <v>1973</v>
+      </c>
+      <c r="QE2">
+        <v>1974</v>
+      </c>
+      <c r="QF2">
+        <v>1975</v>
+      </c>
+      <c r="QG2">
+        <v>1976</v>
+      </c>
+      <c r="QH2">
+        <v>1977</v>
+      </c>
+      <c r="QI2">
+        <v>1978</v>
+      </c>
+      <c r="QJ2">
+        <v>1979</v>
+      </c>
+      <c r="QK2">
+        <v>1980</v>
+      </c>
+      <c r="QL2">
+        <v>1981</v>
+      </c>
+      <c r="QM2">
+        <v>1982</v>
+      </c>
+      <c r="QN2">
+        <v>1983</v>
+      </c>
+      <c r="QO2">
+        <v>1984</v>
+      </c>
+      <c r="QP2">
+        <v>1985</v>
+      </c>
+      <c r="QQ2">
+        <v>1986</v>
+      </c>
+      <c r="QR2">
+        <v>1987</v>
+      </c>
+      <c r="QS2">
+        <v>1988</v>
+      </c>
+      <c r="QT2">
+        <v>1989</v>
+      </c>
+      <c r="QU2">
+        <v>1990</v>
+      </c>
+      <c r="QV2">
+        <v>1991</v>
+      </c>
+      <c r="QW2">
+        <v>1992</v>
+      </c>
+      <c r="QX2">
+        <v>1993</v>
+      </c>
+      <c r="QY2">
+        <v>1994</v>
+      </c>
+      <c r="QZ2">
+        <v>1995</v>
+      </c>
+      <c r="RA2">
+        <v>1996</v>
+      </c>
+      <c r="RB2">
+        <v>1997</v>
+      </c>
+      <c r="RC2">
+        <v>1998</v>
+      </c>
+      <c r="RD2">
+        <v>1999</v>
+      </c>
+      <c r="RE2">
+        <v>2000</v>
+      </c>
+      <c r="RF2">
+        <v>2001</v>
+      </c>
+      <c r="RG2">
+        <v>2002</v>
+      </c>
+      <c r="RH2">
+        <v>2003</v>
+      </c>
+      <c r="RI2">
+        <v>2004</v>
+      </c>
+      <c r="RJ2">
+        <v>2005</v>
+      </c>
+      <c r="RK2">
+        <v>2006</v>
+      </c>
+      <c r="RL2">
+        <v>2007</v>
+      </c>
+      <c r="RM2">
+        <v>2008</v>
+      </c>
+      <c r="RN2">
+        <v>2009</v>
+      </c>
+      <c r="RO2">
+        <v>2010</v>
+      </c>
+      <c r="RP2">
+        <v>2011</v>
+      </c>
+      <c r="RQ2">
+        <v>2012</v>
+      </c>
+      <c r="RR2">
+        <v>2013</v>
+      </c>
+      <c r="RS2">
+        <v>2014</v>
+      </c>
+      <c r="RT2">
+        <v>2015</v>
+      </c>
+      <c r="RU2">
+        <v>2016</v>
+      </c>
+      <c r="RV2">
+        <v>2017</v>
+      </c>
+      <c r="RW2">
+        <v>2018</v>
+      </c>
+      <c r="RX2">
+        <v>2019</v>
+      </c>
+      <c r="RY2">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72422ABD-857E-4B13-A4DD-3030381878EF}">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="8" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1">

</xml_diff>